<commit_message>
Update import template and reader
</commit_message>
<xml_diff>
--- a/navakijwebsite/public/core/download/branches_import_template.xlsx
+++ b/navakijwebsite/public/core/download/branches_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ikidz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ikidz-mbp/Sites/docker-navakij/navakijwebsite/public/core/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AEA63E-392C-004F-9F32-E6402BF02FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EE05EB-B1FD-DA42-BD14-9833DF7AE7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ชื่อ (ไทย)</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>แบรนด์</t>
+  </si>
+  <si>
+    <t>บัตร</t>
+  </si>
+  <si>
+    <t>IPD/OPD</t>
   </si>
 </sst>
 </file>
@@ -138,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -284,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -453,13 +459,14 @@
     <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.1640625" customWidth="1"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.33203125" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,32 +501,38 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2:M1048576" xr:uid="{BFBA15E1-011A-DA42-917F-B8607B46B321}">
-      <formula1>$R$2:$R$3</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N2:O1048576" xr:uid="{BFBA15E1-011A-DA42-917F-B8607B46B321}">
+      <formula1>$T$2:$T$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>